<commit_message>
29-10-2015 Implement User Plan
</commit_message>
<xml_diff>
--- a/New_EmailCampaign/ExcelEmptyTemplate/ExcelTemplate.xlsx
+++ b/New_EmailCampaign/ExcelEmptyTemplate/ExcelTemplate.xlsx
@@ -12,14 +12,14 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet2" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Name</t>
   </si>
@@ -45,10 +45,13 @@
     <t>Country</t>
   </si>
   <si>
-    <t>xxxxx</t>
-  </si>
-  <si>
-    <t>xxxxxxx@gmail.com</t>
+    <t>Dateofbirth</t>
+  </si>
+  <si>
+    <t>XXXXXX</t>
+  </si>
+  <si>
+    <t>xxxxx@xxxx.xxx</t>
   </si>
 </sst>
 </file>
@@ -87,27 +90,12 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -118,11 +106,12 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -404,81 +393,69 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:I4"/>
+  <dimension ref="C3:K4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="C3" sqref="C3:K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="23" customWidth="1"/>
-    <col min="4" max="4" width="17.85546875" customWidth="1"/>
-    <col min="5" max="5" width="15.28515625" customWidth="1"/>
+    <col min="3" max="3" width="20.28515625" customWidth="1"/>
+    <col min="4" max="4" width="32.7109375" customWidth="1"/>
+    <col min="5" max="5" width="25.42578125" customWidth="1"/>
     <col min="6" max="6" width="15.42578125" customWidth="1"/>
-    <col min="7" max="7" width="14.7109375" customWidth="1"/>
-    <col min="8" max="8" width="11.85546875" customWidth="1"/>
-    <col min="9" max="9" width="17.140625" customWidth="1"/>
+    <col min="7" max="7" width="19.140625" customWidth="1"/>
+    <col min="11" max="11" width="14.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B2" s="1" t="s">
+    <row r="3" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="H3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="I3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="J3" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="K3" s="1" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="3" t="s">
+    <row r="4" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-    </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B4" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" s="2"/>
+      <c r="D4" s="3" t="s">
+        <v>10</v>
+      </c>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="4"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C3" r:id="rId1"/>
-    <hyperlink ref="C4" r:id="rId2"/>
+    <hyperlink ref="D4" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>